<commit_message>
Subo notebook con el taller 3 completo y reporte completo con conclusiones para revisión
</commit_message>
<xml_diff>
--- a/Taller 3/tablas.xlsx
+++ b/Taller 3/tablas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1655775e314bd799/Maestría IA Aplicada/Semestre 1/Aprendizaje automático III/Talleres/Taller 2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1655775e314bd799/Maestría IA Aplicada/Semestre 1/Aprendizaje automático III/Talleres/Taller 3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="121" documentId="8_{B1D44CD4-F765-41BB-8147-D381176485D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3C47A0D-F7F4-4DE5-9526-C6FB8097A1DD}"/>
+  <xr:revisionPtr revIDLastSave="132" documentId="8_{B1D44CD4-F765-41BB-8147-D381176485D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92FDA035-49DD-4CE2-B671-5A8AF12B44F8}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="-2475" windowWidth="20730" windowHeight="11040" xr2:uid="{AD1B03CA-9232-4F2D-A5D2-63064345160B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="152">
   <si>
     <t>Modelo</t>
   </si>
@@ -410,9 +410,6 @@
     <t>Ljung-Box</t>
   </si>
   <si>
-    <t>1.29e-30</t>
-  </si>
-  <si>
     <t>Hay autocorrelación</t>
   </si>
   <si>
@@ -422,22 +419,118 @@
     <t>Ljung-Box (res²), Breusch-Pagan</t>
   </si>
   <si>
-    <t>&lt; 0.05 / 0.032</t>
-  </si>
-  <si>
-    <t>Hay heteroscedasticidad</t>
-  </si>
-  <si>
     <t>Normalidad</t>
   </si>
   <si>
     <t>Shapiro-Wilk, Jarque-Bera</t>
   </si>
   <si>
-    <t>0.0056 / 0.014</t>
-  </si>
-  <si>
     <t>No hay normalidad</t>
+  </si>
+  <si>
+    <t>Prueba estadística</t>
+  </si>
+  <si>
+    <t>Resultado</t>
+  </si>
+  <si>
+    <t>P-valor</t>
+  </si>
+  <si>
+    <t>Cumplimiento</t>
+  </si>
+  <si>
+    <t>No autocorrelación</t>
+  </si>
+  <si>
+    <t>Test de Ljung–Box (24 rezagos)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Se </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rechaza H₀</t>
+    </r>
+  </si>
+  <si>
+    <t>&lt; 0.001</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">❌ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>No cumple</t>
+    </r>
+  </si>
+  <si>
+    <t>Existe autocorrelación en los residuos, lo que indica que el modelo no capta toda la dependencia temporal.</t>
+  </si>
+  <si>
+    <t>Test de Shapiro–Wilk</t>
+  </si>
+  <si>
+    <t>Los residuos no siguen una distribución normal, afectando la validez de los intervalos de confianza.</t>
+  </si>
+  <si>
+    <t>Homoscedasticidad</t>
+  </si>
+  <si>
+    <t>Análisis visual (residuos vs tiempo)</t>
+  </si>
+  <si>
+    <t>Varianza estable</t>
+  </si>
+  <si>
+    <t>—</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">✅ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sí cumple</t>
+    </r>
+  </si>
+  <si>
+    <t>La varianza de los residuos se mantiene constante a lo largo del tiempo.</t>
+  </si>
+  <si>
+    <t>1.27e-20</t>
+  </si>
+  <si>
+    <t>0.5658 / 0.1890</t>
+  </si>
+  <si>
+    <t>No hay heteroscedasticidad</t>
+  </si>
+  <si>
+    <t>1.25e-07 / 3.05e-13</t>
   </si>
 </sst>
 </file>
@@ -496,7 +589,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -537,6 +630,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -552,10 +654,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -875,10 +973,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{967B6C11-13F9-4C03-BFC2-EFBD0D58981C}">
-  <dimension ref="C9:K114"/>
+  <dimension ref="C9:M114"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D72" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I76" sqref="I76"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F79" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M93" sqref="M93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -889,9 +987,9 @@
     <col min="6" max="6" width="41.08984375" customWidth="1"/>
     <col min="7" max="7" width="60.1796875" customWidth="1"/>
     <col min="8" max="8" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.90625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.26953125" customWidth="1"/>
-    <col min="11" max="11" width="21.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28" customWidth="1"/>
+    <col min="10" max="10" width="19" customWidth="1"/>
+    <col min="11" max="11" width="23.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="9" spans="4:5" x14ac:dyDescent="0.35">
@@ -1364,7 +1462,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="82" spans="8:11" x14ac:dyDescent="0.35">
+    <row r="82" spans="8:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H82" s="6" t="s">
         <v>118</v>
       </c>
@@ -1378,7 +1476,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="83" spans="8:11" x14ac:dyDescent="0.35">
+    <row r="83" spans="8:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H83" s="6" t="s">
         <v>122</v>
       </c>
@@ -1386,38 +1484,118 @@
         <v>123</v>
       </c>
       <c r="J83" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="K83" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="K83" s="13" t="s">
+    </row>
+    <row r="84" spans="8:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H84" s="6" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="84" spans="8:11" x14ac:dyDescent="0.35">
-      <c r="H84" s="6" t="s">
+      <c r="I84" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="I84" s="13" t="s">
+      <c r="J84" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="K84" s="13" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="85" spans="8:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H85" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="J84" s="4" t="s">
+      <c r="I85" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="K84" s="13" t="s">
+      <c r="J85" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="K85" s="13" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="85" spans="8:11" x14ac:dyDescent="0.35">
-      <c r="H85" s="6" t="s">
+    <row r="92" spans="8:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="H92" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="I92" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="I85" s="13" t="s">
+      <c r="J92" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="J85" s="4" t="s">
+      <c r="K92" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="K85" s="13" t="s">
+      <c r="L92" s="14" t="s">
         <v>133</v>
+      </c>
+      <c r="M92" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="93" spans="8:13" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="H93" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="I93" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="J93" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="K93" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="L93" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="M93" s="15" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="94" spans="8:13" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="H94" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="I94" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="J94" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="K94" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="L94" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="M94" s="15" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="95" spans="8:13" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="H95" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="I95" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="J95" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="K95" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="L95" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="M95" s="15" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="105" spans="9:11" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Subo notebook con taller 3 completo e informe, hay un notebook con pruebas de transformaciones
</commit_message>
<xml_diff>
--- a/Taller 3/tablas.xlsx
+++ b/Taller 3/tablas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1655775e314bd799/Maestría IA Aplicada/Semestre 1/Aprendizaje automático III/Talleres/Taller 3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="132" documentId="8_{B1D44CD4-F765-41BB-8147-D381176485D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92FDA035-49DD-4CE2-B671-5A8AF12B44F8}"/>
+  <xr:revisionPtr revIDLastSave="143" documentId="8_{B1D44CD4-F765-41BB-8147-D381176485D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC3F681A-8915-4186-B280-E3030F95059D}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="-2475" windowWidth="20730" windowHeight="11040" xr2:uid="{AD1B03CA-9232-4F2D-A5D2-63064345160B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="170">
   <si>
     <t>Modelo</t>
   </si>
@@ -531,6 +531,60 @@
   </si>
   <si>
     <t>1.25e-07 / 3.05e-13</t>
+  </si>
+  <si>
+    <t>10866.35</t>
+  </si>
+  <si>
+    <t>10529.82</t>
+  </si>
+  <si>
+    <t>11202.87</t>
+  </si>
+  <si>
+    <t>10884.31</t>
+  </si>
+  <si>
+    <t>10495.27</t>
+  </si>
+  <si>
+    <t>11273.35</t>
+  </si>
+  <si>
+    <t>10902.10</t>
+  </si>
+  <si>
+    <t>10491.03</t>
+  </si>
+  <si>
+    <t>11313.16</t>
+  </si>
+  <si>
+    <t>10919.82</t>
+  </si>
+  <si>
+    <t>10495.52</t>
+  </si>
+  <si>
+    <t>11344.12</t>
+  </si>
+  <si>
+    <t>10937.50</t>
+  </si>
+  <si>
+    <t>10503.14</t>
+  </si>
+  <si>
+    <t>11371.87</t>
+  </si>
+  <si>
+    <t>10955.17</t>
+  </si>
+  <si>
+    <t>10512.07</t>
+  </si>
+  <si>
+    <t>11398.28</t>
   </si>
 </sst>
 </file>
@@ -654,6 +708,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -975,8 +1033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{967B6C11-13F9-4C03-BFC2-EFBD0D58981C}">
   <dimension ref="C9:M114"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F79" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M93" sqref="M93"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A47" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -984,7 +1042,7 @@
     <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.08984375" customWidth="1"/>
+    <col min="6" max="6" width="14.6328125" customWidth="1"/>
     <col min="7" max="7" width="60.1796875" customWidth="1"/>
     <col min="8" max="8" width="18.26953125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="28" customWidth="1"/>
@@ -1378,6 +1436,104 @@
         <v>62</v>
       </c>
     </row>
+    <row r="59" spans="3:6" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C59" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="60" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C60" s="7">
+        <v>43647</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="E60" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="F60" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="61" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C61" s="7">
+        <v>43678</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="E61" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="F61" s="8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="62" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C62" s="7">
+        <v>43709</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="E62" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="F62" s="8" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="63" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C63" s="7">
+        <v>43739</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="E63" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="F63" s="8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="64" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C64" s="7">
+        <v>43770</v>
+      </c>
+      <c r="D64" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="E64" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="F64" s="8" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="65" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C65" s="7">
+        <v>43800</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="E65" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="F65" s="8" t="s">
+        <v>169</v>
+      </c>
+    </row>
     <row r="68" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C68" s="1" t="s">
         <v>0</v>

</xml_diff>